<commit_message>
added footer/style. uploaded most of the pics
</commit_message>
<xml_diff>
--- a/utilities/web_project_Scrum.xlsx
+++ b/utilities/web_project_Scrum.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\kasmir\src\kasmir_moilanen\team1web_project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\kasmir\src\kasmir_moilanen\team1web_project\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907D7613-D731-4096-BC73-961313399B63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD188BFB-FB1A-43B4-913B-F2F199E6E6DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12804" yWindow="2532" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ListOfFeatures" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="62">
-  <si>
-    <t>Product Backlog - Project Title (List of your features)</t>
-  </si>
   <si>
     <t>User Stories / List of features</t>
   </si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>divider</t>
+  </si>
+  <si>
+    <t>Product Backlog - Gym one (List of your features)</t>
   </si>
 </sst>
 </file>
@@ -1518,8 +1518,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B1000"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1531,40 +1531,40 @@
     <col min="6" max="26" width="8.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:2" ht="31.8" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A1" s="11" t="s">
-        <v>0</v>
+        <v>61</v>
       </c>
       <c r="B1" s="12"/>
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1572,12 +1572,12 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1588,27 +1588,27 @@
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1616,27 +1616,27 @@
     </row>
     <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1644,27 +1644,27 @@
     </row>
     <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2708,7 +2708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
@@ -2723,7 +2723,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -2741,16 +2741,16 @@
     </row>
     <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>6</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -2765,7 +2765,7 @@
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
@@ -2783,14 +2783,14 @@
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -2805,14 +2805,14 @@
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>53</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>54</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -2827,14 +2827,14 @@
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -2849,14 +2849,14 @@
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -2871,14 +2871,14 @@
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>59</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>60</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -2893,14 +2893,14 @@
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -2915,7 +2915,7 @@
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
@@ -2933,7 +2933,7 @@
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -2951,7 +2951,7 @@
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -2969,7 +2969,7 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -2987,7 +2987,7 @@
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -3005,7 +3005,7 @@
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
@@ -3023,7 +3023,7 @@
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -3041,7 +3041,7 @@
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -3059,7 +3059,7 @@
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -3077,7 +3077,7 @@
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -3095,7 +3095,7 @@
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
@@ -3113,7 +3113,7 @@
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -3131,7 +3131,7 @@
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -3149,7 +3149,7 @@
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -3167,7 +3167,7 @@
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -3185,7 +3185,7 @@
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
@@ -3203,7 +3203,7 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -3221,7 +3221,7 @@
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -3239,7 +3239,7 @@
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -3257,7 +3257,7 @@
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -3275,7 +3275,7 @@
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -4290,7 +4290,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -4308,16 +4308,16 @@
     </row>
     <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>6</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -4332,7 +4332,7 @@
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
@@ -4350,16 +4350,16 @@
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="9">
         <v>2</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>9</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>10</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -4374,13 +4374,13 @@
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="9">
         <v>2</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="6"/>
@@ -4396,13 +4396,13 @@
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="9">
         <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="6"/>
@@ -4418,13 +4418,13 @@
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="9">
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="6"/>
@@ -4440,7 +4440,7 @@
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -4458,7 +4458,7 @@
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -4476,7 +4476,7 @@
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -4494,7 +4494,7 @@
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -4512,7 +4512,7 @@
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -4530,7 +4530,7 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
@@ -4548,7 +4548,7 @@
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -4566,7 +4566,7 @@
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -4584,7 +4584,7 @@
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -4602,7 +4602,7 @@
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -4620,7 +4620,7 @@
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
@@ -4638,7 +4638,7 @@
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -4656,7 +4656,7 @@
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -4674,7 +4674,7 @@
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -4692,7 +4692,7 @@
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -4710,7 +4710,7 @@
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
@@ -4728,7 +4728,7 @@
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -4746,7 +4746,7 @@
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -4764,7 +4764,7 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -4782,7 +4782,7 @@
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -4800,7 +4800,7 @@
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -5815,7 +5815,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -5833,16 +5833,16 @@
     </row>
     <row r="2" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>5</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>6</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -5857,7 +5857,7 @@
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
@@ -5875,16 +5875,16 @@
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4" s="9">
         <v>2</v>
       </c>
       <c r="C4" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="9" t="s">
         <v>9</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>10</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -5899,13 +5899,13 @@
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B5" s="9">
         <v>2</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="6"/>
@@ -5921,13 +5921,13 @@
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="9">
         <v>4</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="6"/>
@@ -5943,13 +5943,13 @@
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B7" s="9">
         <v>2</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D7" s="9"/>
       <c r="E7" s="6"/>
@@ -5965,7 +5965,7 @@
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -5983,7 +5983,7 @@
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9"/>
@@ -6001,7 +6001,7 @@
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B10" s="9"/>
       <c r="C10" s="9"/>
@@ -6019,7 +6019,7 @@
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -6037,7 +6037,7 @@
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -6055,7 +6055,7 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
@@ -6073,7 +6073,7 @@
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -6091,7 +6091,7 @@
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -6109,7 +6109,7 @@
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -6127,7 +6127,7 @@
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -6145,7 +6145,7 @@
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
@@ -6163,7 +6163,7 @@
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -6181,7 +6181,7 @@
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -6199,7 +6199,7 @@
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -6217,7 +6217,7 @@
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -6235,7 +6235,7 @@
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
@@ -6253,7 +6253,7 @@
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -6271,7 +6271,7 @@
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -6289,7 +6289,7 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -6307,7 +6307,7 @@
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -6325,7 +6325,7 @@
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>

</xml_diff>

<commit_message>
added user pages and styles
working on displaying page content from db's
</commit_message>
<xml_diff>
--- a/utilities/web_project_Scrum.xlsx
+++ b/utilities/web_project_Scrum.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\kasmir\src\kasmir_moilanen\team1web_project\utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE234C35-D5A7-4B8E-BBBC-423FF8E99D68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF336C9C-E372-45EC-85EB-7CE10F63CF4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ListOfFeatures" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="67">
   <si>
     <t>User Stories / List of features</t>
   </si>
@@ -49,24 +49,6 @@
   </si>
   <si>
     <t>User Story/ Feature #1</t>
-  </si>
-  <si>
-    <t>Task : Make a list of categories of products</t>
-  </si>
-  <si>
-    <t>Pekka</t>
-  </si>
-  <si>
-    <t>Ongoing</t>
-  </si>
-  <si>
-    <t>Task : List products based on categories</t>
-  </si>
-  <si>
-    <t>Task : Search products</t>
-  </si>
-  <si>
-    <t>Task: Display products</t>
   </si>
   <si>
     <t>User Story #2</t>
@@ -97,15 +79,6 @@
   </si>
   <si>
     <t>User Story #1</t>
-  </si>
-  <si>
-    <t>Juha</t>
-  </si>
-  <si>
-    <t>Johanna</t>
-  </si>
-  <si>
-    <t>Markku</t>
   </si>
   <si>
     <t>Sprint Backlog : Sprint 3 (Feb 21 - Feb 25)</t>
@@ -229,6 +202,33 @@
   </si>
   <si>
     <t>contact.php</t>
+  </si>
+  <si>
+    <t>testing</t>
+  </si>
+  <si>
+    <t>all</t>
+  </si>
+  <si>
+    <t>finalizing the project</t>
+  </si>
+  <si>
+    <t>fixing user stuff and links</t>
+  </si>
+  <si>
+    <t>gallery</t>
+  </si>
+  <si>
+    <t>blog</t>
+  </si>
+  <si>
+    <t>displayinng stuff on frontend(user)</t>
+  </si>
+  <si>
+    <t>fixing broken stuff and testing that it works</t>
+  </si>
+  <si>
+    <t>trainer needs img</t>
   </si>
 </sst>
 </file>
@@ -1548,7 +1548,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="31.8" customHeight="1" x14ac:dyDescent="0.65">
       <c r="A1" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="B1" s="12"/>
     </row>
@@ -1559,27 +1559,27 @@
     </row>
     <row r="3" spans="1:2" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1587,12 +1587,12 @@
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1603,27 +1603,27 @@
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1631,27 +1631,27 @@
     </row>
     <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -1659,27 +1659,27 @@
     </row>
     <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="2" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="2" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
@@ -2798,14 +2798,14 @@
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -2820,14 +2820,14 @@
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -2842,14 +2842,14 @@
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -2864,14 +2864,14 @@
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -2886,14 +2886,14 @@
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B8" s="9"/>
       <c r="C8" s="9" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="E8" s="6"/>
       <c r="F8" s="6"/>
@@ -2908,14 +2908,14 @@
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -2930,7 +2930,7 @@
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B10" s="7"/>
       <c r="C10" s="8"/>
@@ -2948,7 +2948,7 @@
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="9"/>
@@ -2966,7 +2966,7 @@
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -2984,7 +2984,7 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -3002,7 +3002,7 @@
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -3020,7 +3020,7 @@
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B15" s="7"/>
       <c r="C15" s="8"/>
@@ -3038,7 +3038,7 @@
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -3056,7 +3056,7 @@
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -3074,7 +3074,7 @@
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -3092,7 +3092,7 @@
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -3110,7 +3110,7 @@
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B20" s="7"/>
       <c r="C20" s="8"/>
@@ -3128,7 +3128,7 @@
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -3146,7 +3146,7 @@
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -3164,7 +3164,7 @@
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
@@ -3182,7 +3182,7 @@
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B25" s="7"/>
       <c r="C25" s="8"/>
@@ -3218,7 +3218,7 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -3236,7 +3236,7 @@
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -3254,7 +3254,7 @@
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="9"/>
@@ -3272,7 +3272,7 @@
     </row>
     <row r="29" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="9"/>
@@ -3290,7 +3290,7 @@
     </row>
     <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B30" s="10"/>
       <c r="C30" s="10"/>
@@ -4292,8 +4292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -4307,7 +4307,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -4328,7 +4328,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>
@@ -4349,7 +4349,7 @@
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
@@ -4367,11 +4367,11 @@
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>58</v>
@@ -4389,14 +4389,14 @@
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="9" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -4411,14 +4411,14 @@
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B6" s="9"/>
       <c r="C6" s="9" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -4433,14 +4433,14 @@
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B7" s="9"/>
       <c r="C7" s="9" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -4471,14 +4471,14 @@
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B9" s="9"/>
       <c r="C9" s="9" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>58</v>
+        <v>43</v>
       </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
@@ -4541,7 +4541,7 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
@@ -4559,7 +4559,7 @@
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -4577,7 +4577,7 @@
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -4595,7 +4595,7 @@
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -4613,7 +4613,7 @@
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -4631,7 +4631,7 @@
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
@@ -4649,7 +4649,7 @@
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -4667,7 +4667,7 @@
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -4685,7 +4685,7 @@
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -4703,7 +4703,7 @@
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -4721,7 +4721,7 @@
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
@@ -4739,7 +4739,7 @@
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -4757,7 +4757,7 @@
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -4775,7 +4775,7 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -4793,7 +4793,7 @@
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -4811,7 +4811,7 @@
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>
@@ -5813,8 +5813,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:N1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:N1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -5828,7 +5828,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="14"/>
@@ -5849,7 +5849,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>
@@ -5870,7 +5870,7 @@
     </row>
     <row r="3" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B3" s="7"/>
       <c r="C3" s="8"/>
@@ -5888,16 +5888,14 @@
     </row>
     <row r="4" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="9">
-        <v>2</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="B4" s="9"/>
       <c r="C4" s="9" t="s">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>9</v>
+        <v>49</v>
       </c>
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
@@ -5912,15 +5910,15 @@
     </row>
     <row r="5" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="9">
-        <v>2</v>
-      </c>
+        <v>65</v>
+      </c>
+      <c r="B5" s="9"/>
       <c r="C5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="D5" s="9"/>
+        <v>59</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
       <c r="G5" s="6"/>
@@ -5934,15 +5932,15 @@
     </row>
     <row r="6" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="9">
-        <v>4</v>
-      </c>
+        <v>66</v>
+      </c>
+      <c r="B6" s="9"/>
       <c r="C6" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="9"/>
+        <v>47</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
       <c r="G6" s="6"/>
@@ -5956,15 +5954,15 @@
     </row>
     <row r="7" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="9">
-        <v>2</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="B7" s="9"/>
       <c r="C7" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="D7" s="9"/>
+        <v>59</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
       <c r="G7" s="6"/>
@@ -5978,7 +5976,7 @@
     </row>
     <row r="8" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="7" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="B8" s="7"/>
       <c r="C8" s="8"/>
@@ -5996,11 +5994,15 @@
     </row>
     <row r="9" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>14</v>
+        <v>62</v>
       </c>
       <c r="B9" s="9"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="9"/>
+      <c r="C9" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="E9" s="6"/>
       <c r="F9" s="6"/>
       <c r="G9" s="6"/>
@@ -6014,11 +6016,15 @@
     </row>
     <row r="10" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>15</v>
+        <v>63</v>
       </c>
       <c r="B10" s="9"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
+      <c r="C10" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="E10" s="6"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
@@ -6032,11 +6038,15 @@
     </row>
     <row r="11" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>14</v>
+        <v>64</v>
       </c>
       <c r="B11" s="9"/>
-      <c r="C11" s="9"/>
-      <c r="D11" s="9"/>
+      <c r="C11" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>49</v>
+      </c>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
       <c r="G11" s="6"/>
@@ -6049,9 +6059,7 @@
       <c r="N11" s="6"/>
     </row>
     <row r="12" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="9" t="s">
-        <v>14</v>
-      </c>
+      <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
@@ -6068,7 +6076,7 @@
     </row>
     <row r="13" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="7" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B13" s="7"/>
       <c r="C13" s="8"/>
@@ -6086,7 +6094,7 @@
     </row>
     <row r="14" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
@@ -6104,7 +6112,7 @@
     </row>
     <row r="15" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
@@ -6122,7 +6130,7 @@
     </row>
     <row r="16" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="9"/>
@@ -6140,7 +6148,7 @@
     </row>
     <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -6158,7 +6166,7 @@
     </row>
     <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B18" s="7"/>
       <c r="C18" s="8"/>
@@ -6176,7 +6184,7 @@
     </row>
     <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -6194,7 +6202,7 @@
     </row>
     <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B20" s="9"/>
       <c r="C20" s="9"/>
@@ -6212,7 +6220,7 @@
     </row>
     <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B21" s="9"/>
       <c r="C21" s="9"/>
@@ -6230,7 +6238,7 @@
     </row>
     <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B22" s="9"/>
       <c r="C22" s="9"/>
@@ -6248,7 +6256,7 @@
     </row>
     <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="7" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B23" s="7"/>
       <c r="C23" s="8"/>
@@ -6266,7 +6274,7 @@
     </row>
     <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="9"/>
@@ -6284,7 +6292,7 @@
     </row>
     <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
@@ -6302,7 +6310,7 @@
     </row>
     <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
@@ -6320,7 +6328,7 @@
     </row>
     <row r="27" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="9" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="9"/>
@@ -6338,7 +6346,7 @@
     </row>
     <row r="28" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="B28" s="10"/>
       <c r="C28" s="10"/>

</xml_diff>